<commit_message>
#1660 Renamed schema files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="5AFBEB918A5A" lockStructure="1"/>
+  <workbookProtection workbookPassword="43AA0DCB4081" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="5AFBEB918A5A"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="43AA0DCB4081"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="5AFBEB918A5A"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="43AA0DCB4081"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
#1643 regenerated output files
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="43AA0DCB4081" lockStructure="1"/>
+  <workbookProtection workbookPassword="89BE88FFB63" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,12 +31843,12 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="43AA0DCB4081"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="89BE88FFB63"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
     </dataValidation>
-    <dataValidation sqref="C2:C3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Y/N" error="Must be 'Y' or 'N'" type="list">
+    <dataValidation sqref="C2:C3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Y/N" error="Must be 'Y' or 'N'" type="list" errorStyle="stop">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -31884,9 +31884,9 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="43AA0DCB4081"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="89BE88FFB63"/>
   <dataValidations count="1">
-    <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with only twelve characters" type="textLength" operator="equal">
+    <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with 12 characters" type="textLength" operator="equal">
       <formula1>12</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated simple case to fit requirement changes
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="87FDBFE5DB1" lockStructure="1"/>
+  <workbookProtection workbookPassword="27E9D5101E5E" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="87FDBFE5DB1"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27E9D5101E5E"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="87FDBFE5DB1"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27E9D5101E5E"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with 12 characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>

<commit_message>
Updated validation rules around clusterName/stateClusterName/OtherClusterName
</commit_message>
<xml_diff>
--- a/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
+++ b/backend/schemas/output/excel/xlsx/corrective-action-plan-workbook.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection workbookPassword="27E9D5101E5E" lockStructure="1"/>
+  <workbookProtection workbookPassword="10E0DD41A1EA" lockStructure="1"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
@@ -31843,7 +31843,7 @@
       <c r="C2999" s="2" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27E9D5101E5E"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10E0DD41A1EA"/>
   <dataValidations count="2">
     <dataValidation sqref="A2:A3000" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Reference number" error="Expecting a value in the format YYYY-NNN, where YYYY is a year and NNN a three digit number (e.g. 2023-001)" type="custom">
       <formula1>=OR(ISBLANK($A2), AND(LEN($A2) = 8, LEFT($A2, 2) = "20", ISNUMBER(MID($A2, 3, 2) * 1), MID($A2, 5, 1) = "-", ISNUMBER(RIGHT($A2, 3) * 1)))</formula1>
@@ -31884,7 +31884,7 @@
       <c r="A2" s="3" t="n"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="27E9D5101E5E"/>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" sheet="1" objects="0" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="0" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" formatRows="1" sort="1" password="10E0DD41A1EA"/>
   <dataValidations count="1">
     <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="1" allowBlank="1" errorTitle="Must be length of 12" error="Expecting something with 12 characters" type="textLength" operator="equal">
       <formula1>12</formula1>

</xml_diff>